<commit_message>
ja en nee vragen voor mannelijke kant en logboek ingevoerd
</commit_message>
<xml_diff>
--- a/Documentatie/Logboek arch 1 final week.xlsx
+++ b/Documentatie/Logboek arch 1 final week.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31620\OneDrive - Hogeschool Rotterdam\Documenten\Hogeschool Rotterdam\Arch 1 finalweek\One-piece-game\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EB2E8C-C8A2-4D8B-809A-79847B2F1C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7081AEB-DD62-48C0-894B-3EF3C1E02818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>🤔 Why keep a logbook?</t>
   </si>
@@ -195,9 +195,6 @@
     <t>Maandag 29 september</t>
   </si>
   <si>
-    <t>Begonnen met plan van aanpak en planning over heel basecamp en begonnen met teksten verzinnen voor tekst-basegame.</t>
-  </si>
-  <si>
     <t>5 uur</t>
   </si>
   <si>
@@ -210,7 +207,31 @@
     <t>2 uur en 50 minuten</t>
   </si>
   <si>
-    <t>Begonnen met flowchart voor de mannelijke characters.</t>
+    <t>flowchart, plan van aanpak, code schrijven</t>
+  </si>
+  <si>
+    <t>5.5 uur</t>
+  </si>
+  <si>
+    <t>3 uur</t>
+  </si>
+  <si>
+    <t>Dinsdag: 5 uur en 50 minuten</t>
+  </si>
+  <si>
+    <t>Woensdag 1 oktober</t>
+  </si>
+  <si>
+    <t>code schrijven en scrumboard</t>
+  </si>
+  <si>
+    <t>Woensdag: 5 uur 50 minuten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flowchart, plan van aanpak, code schrijven en teksten </t>
+  </si>
+  <si>
+    <t>Plan van aanpak, planning, scrumboard en teksten</t>
   </si>
 </sst>
 </file>
@@ -389,7 +410,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -417,35 +438,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="12" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="20" fontId="10" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="20" fontId="13" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="20" fontId="11" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -483,14 +480,51 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="11" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1784,16 +1818,16 @@
   <dimension ref="B1:G994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="20.8984375" customWidth="1"/>
     <col min="3" max="4" width="10.3984375" customWidth="1"/>
-    <col min="5" max="5" width="17.8984375" style="18" customWidth="1"/>
+    <col min="5" max="5" width="17.8984375" style="13" customWidth="1"/>
     <col min="6" max="6" width="68.59765625" customWidth="1"/>
-    <col min="7" max="7" width="13.09765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="14.4" x14ac:dyDescent="0.3">
@@ -1809,7 +1843,7 @@
       <c r="D2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="14" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -1822,399 +1856,427 @@
     <row r="3" spans="2:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B3" s="9"/>
     </row>
-    <row r="4" spans="2:7" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+    <row r="4" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="15">
         <v>0.39583333333333331</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="15">
         <v>0.60416666666666663</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="26" t="s">
+    </row>
+    <row r="5" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B5" s="19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B5" s="27" t="s">
+      <c r="C5" s="20">
+        <v>0.40277777777777779</v>
+      </c>
+      <c r="D5" s="20">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="28">
-        <v>0.40277777777777779</v>
+      <c r="F5" s="17" t="s">
+        <v>35</v>
       </c>
-      <c r="D5" s="28">
+      <c r="G5" s="40" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="23">
         <v>0.52083333333333337</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="D6" s="24">
+        <v>0.6875</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B7" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="24">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D7" s="24">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E7" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="30"/>
-    </row>
-    <row r="6" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="32"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="35"/>
-    </row>
-    <row r="7" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B7" s="36"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="35"/>
+      <c r="F7" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="8" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="35"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="22"/>
     </row>
     <row r="9" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="35"/>
+      <c r="B9" s="27"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B10" s="36"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="37"/>
-      <c r="G10" s="35"/>
+      <c r="B10" s="27"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="35"/>
+      <c r="B11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B12" s="36"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="35"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B13" s="36"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="35"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="22"/>
     </row>
     <row r="14" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="33"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="35"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="22"/>
     </row>
     <row r="15" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B15" s="36"/>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="35"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="22"/>
     </row>
     <row r="16" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B16" s="14"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="15"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="30"/>
     </row>
     <row r="17" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="15"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="30"/>
     </row>
     <row r="18" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="15"/>
+      <c r="B18" s="29"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="30"/>
     </row>
     <row r="19" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="15"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="30"/>
     </row>
     <row r="20" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B20" s="14"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="15"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="30"/>
     </row>
     <row r="21" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B21" s="14"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="13"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="32"/>
     </row>
     <row r="22" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B22" s="14"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="13"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
     </row>
     <row r="23" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="15"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="30"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="30"/>
     </row>
     <row r="24" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="13"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="30"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="32"/>
     </row>
     <row r="25" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B25" s="14"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="15"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="30"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="30"/>
     </row>
     <row r="26" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="13"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="32"/>
     </row>
     <row r="27" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B27" s="14"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="13"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="32"/>
     </row>
     <row r="28" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B28" s="14"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="13"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="32"/>
     </row>
     <row r="29" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B29" s="14"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="16"/>
+      <c r="B29" s="29"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="33"/>
     </row>
     <row r="30" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B30" s="14"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="13"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="32"/>
     </row>
     <row r="31" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B31" s="14"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="13"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="32"/>
     </row>
     <row r="32" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B32" s="17"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="13"/>
+      <c r="B32" s="35"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="36"/>
+      <c r="F32" s="32"/>
     </row>
     <row r="33" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B33" s="17"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="13"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="36"/>
+      <c r="F33" s="32"/>
     </row>
     <row r="34" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B34" s="17"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="13"/>
+      <c r="B34" s="35"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="36"/>
+      <c r="F34" s="32"/>
     </row>
     <row r="35" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B35" s="17"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="13"/>
+      <c r="B35" s="35"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="32"/>
     </row>
     <row r="36" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B36" s="14"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="13"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="32"/>
     </row>
     <row r="37" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B37" s="17"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="13"/>
+      <c r="B37" s="35"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="36"/>
+      <c r="F37" s="32"/>
     </row>
     <row r="38" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B38" s="17"/>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="13"/>
+      <c r="B38" s="35"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="36"/>
+      <c r="F38" s="32"/>
     </row>
     <row r="39" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B39" s="17"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="22"/>
-      <c r="F39" s="13"/>
+      <c r="B39" s="35"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="32"/>
     </row>
     <row r="40" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B40" s="17"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="22"/>
-      <c r="F40" s="13"/>
+      <c r="B40" s="35"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="32"/>
     </row>
     <row r="41" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B41" s="17"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="13"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="32"/>
     </row>
     <row r="42" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B42" s="17"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="13"/>
+      <c r="B42" s="35"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="36"/>
+      <c r="F42" s="32"/>
     </row>
     <row r="43" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B43" s="17"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="13"/>
+      <c r="B43" s="35"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="36"/>
+      <c r="F43" s="32"/>
     </row>
     <row r="44" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B44" s="17"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="22"/>
-      <c r="F44" s="13"/>
+      <c r="B44" s="35"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="32"/>
     </row>
     <row r="45" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B45" s="17"/>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="13"/>
+      <c r="B45" s="35"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="32"/>
     </row>
     <row r="46" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B46" s="17"/>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="13"/>
+      <c r="B46" s="35"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="32"/>
     </row>
     <row r="47" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B47" s="17"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="13"/>
+      <c r="B47" s="35"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="32"/>
     </row>
     <row r="48" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B48" s="14"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="13"/>
+      <c r="B48" s="29"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="32"/>
     </row>
     <row r="49" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B49" s="14"/>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="13"/>
+      <c r="B49" s="29"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="32"/>
     </row>
     <row r="50" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B50" s="17"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="22"/>
-      <c r="F50" s="13"/>
+      <c r="B50" s="35"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="32"/>
     </row>
     <row r="51" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B51" s="17"/>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="22"/>
-      <c r="F51" s="13"/>
+      <c r="B51" s="35"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="32"/>
     </row>
     <row r="52" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B52" s="17"/>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="22"/>
-      <c r="F52" s="13"/>
+      <c r="B52" s="35"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="36"/>
+      <c r="F52" s="32"/>
     </row>
     <row r="53" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B53" s="14"/>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="13"/>
+      <c r="B53" s="29"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="32"/>
     </row>
     <row r="54" spans="2:6" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B54" s="14"/>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="20"/>
-      <c r="F54" s="13"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="32"/>
     </row>
     <row r="55" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B55" s="9"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="38"/>
     </row>
     <row r="56" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B56" s="9"/>
@@ -5035,6 +5097,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5108,21 +5171,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010051CD740541D4B64EA1D3B007F5EE4BC0" ma:contentTypeVersion="3" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="3ab1eaadcc6d0267840b762a82710713">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f3454686-2221-44b3-8f28-41e6911d9062" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e7c55293e0639ab65759325b37ae43e4" ns2:_="">
     <xsd:import namespace="f3454686-2221-44b3-8f28-41e6911d9062"/>
@@ -5260,24 +5308,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14BB4D6E-C856-4503-A5F5-487F247D347A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78E03D4F-D06B-40C1-A53D-F1DEB199C8A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{056185FF-4622-4DC5-8DE7-928B36226CD5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5293,4 +5339,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14BB4D6E-C856-4503-A5F5-487F247D347A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78E03D4F-D06B-40C1-A53D-F1DEB199C8A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update logboek dag 5
</commit_message>
<xml_diff>
--- a/Documentatie/Logboek arch 1 final week.xlsx
+++ b/Documentatie/Logboek arch 1 final week.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\31620\OneDrive - Hogeschool Rotterdam\Documenten\Hogeschool Rotterdam\Arch 1 finalweek\One-piece-game\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{46521937-72D7-4BBA-8F0C-5793668FCF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26C069F5-95C2-469A-BF1E-F1EC036F8550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>🤔 Why keep a logbook?</t>
   </si>
@@ -213,9 +213,6 @@
     <t>5.5 uur</t>
   </si>
   <si>
-    <t>code schrijven en scrumboard</t>
-  </si>
-  <si>
     <t>Woensdag: 5 uur 50 minuten</t>
   </si>
   <si>
@@ -240,10 +237,25 @@
     <t>Dondergdag 2 oktober</t>
   </si>
   <si>
-    <t xml:space="preserve">code herschrijven en testen </t>
+    <t xml:space="preserve">Donderdag:  5 uur </t>
   </si>
   <si>
-    <t xml:space="preserve">Donderdag:  5 uur </t>
+    <t>Vrijdag 3 oktober</t>
+  </si>
+  <si>
+    <t>1 uur</t>
+  </si>
+  <si>
+    <t>Vrijdag: 1 uur</t>
+  </si>
+  <si>
+    <t>Afronding challenge week en project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code herschrijven en testen </t>
+  </si>
+  <si>
+    <t>Code schrijven en scrumboard</t>
   </si>
 </sst>
 </file>
@@ -1871,7 +1883,7 @@
   <dimension ref="B1:G994"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1981,15 +1993,15 @@
         <v>29</v>
       </c>
       <c r="F7" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="37" t="s">
         <v>30</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B8" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" s="24">
         <v>0.40625</v>
@@ -2001,19 +2013,31 @@
         <v>19</v>
       </c>
       <c r="F8" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="37" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="B9" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="C9" s="24">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="D9" s="24">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E9" s="39" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="22"/>
+      <c r="F9" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="37" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B10" s="27"/>
@@ -2057,7 +2081,7 @@
     </row>
     <row r="15" spans="2:7" s="12" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B15" s="27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="40"/>
       <c r="D15" s="28"/>
@@ -5180,7 +5204,7 @@
   <sheetData>
     <row r="3" spans="2:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5210,22 +5234,22 @@
     </row>
     <row r="11" spans="2:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="2:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -5234,20 +5258,20 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="a2ab80be-5373-4572-a855-5468ce13c95a" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="a2ab80be-5373-4572-a855-5468ce13c95a" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5427,6 +5451,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78E03D4F-D06B-40C1-A53D-F1DEB199C8A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{14BB4D6E-C856-4503-A5F5-487F247D347A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -5438,14 +5470,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="a2ab80be-5373-4572-a855-5468ce13c95a"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{78E03D4F-D06B-40C1-A53D-F1DEB199C8A7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>